<commit_message>
Profile and ModelCode update
</commit_message>
<xml_diff>
--- a/9_ModelCode.xlsx
+++ b/9_ModelCode.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="abstract-concrete" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="attributes" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Outage::OutageSchedule</t>
   </si>
@@ -39,7 +39,106 @@
     <t>Core::RegularIntervalSchedule</t>
   </si>
   <si>
-    <t>Core::RegularIntervalTimePoint</t>
+    <t>Core::RegularTimePoint</t>
+  </si>
+  <si>
+    <t>Core::IdentifiedObject</t>
+  </si>
+  <si>
+    <t>Core::PowerSystemResource</t>
+  </si>
+  <si>
+    <t>Core::Equipment</t>
+  </si>
+  <si>
+    <t>Core::ConductingEquipment</t>
+  </si>
+  <si>
+    <t>Wires::Switch</t>
+  </si>
+  <si>
+    <t>Core::BasicIntervalSchedule</t>
+  </si>
+  <si>
+    <t>Core::IrregularIntervalSchedule</t>
+  </si>
+  <si>
+    <t>IdentifiedObject</t>
+  </si>
+  <si>
+    <t>aliasName: String</t>
+  </si>
+  <si>
+    <t>mRID: String</t>
+  </si>
+  <si>
+    <t>name: String</t>
+  </si>
+  <si>
+    <t>BasicIntervalSchedule</t>
+  </si>
+  <si>
+    <t>startTime: DateTime</t>
+  </si>
+  <si>
+    <t>value1Multiplier: UnitMultiplier</t>
+  </si>
+  <si>
+    <t>value1Unit: UnitSymbol</t>
+  </si>
+  <si>
+    <t>value2Multiplier: UnitMultiplier</t>
+  </si>
+  <si>
+    <t>value2Unit: UnitSymbol</t>
+  </si>
+  <si>
+    <t>SwitchingOperation</t>
+  </si>
+  <si>
+    <t>newState: SwitchState</t>
+  </si>
+  <si>
+    <t>operationTime: DateTime</t>
+  </si>
+  <si>
+    <t>OutageSchedule: REFERENCE</t>
+  </si>
+  <si>
+    <t>IrregularTimePoint</t>
+  </si>
+  <si>
+    <t>time: Secounds</t>
+  </si>
+  <si>
+    <t>value1: Float</t>
+  </si>
+  <si>
+    <t>value2: Float</t>
+  </si>
+  <si>
+    <t>IntervalSchedule: REFERENCE</t>
+  </si>
+  <si>
+    <t>RegularIntervalSchedule</t>
+  </si>
+  <si>
+    <t>endTime: DateTime</t>
+  </si>
+  <si>
+    <t>timeStep: Secounds</t>
+  </si>
+  <si>
+    <t>RegularTimePoint</t>
+  </si>
+  <si>
+    <t>sequenceNumber: Integer</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>SwitchingOperations: REFERENCE</t>
   </si>
 </sst>
 </file>
@@ -426,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,33 +546,56 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
       <c r="B7" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -484,12 +606,123 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>